<commit_message>
Update MCU TorqueControl CAN协议V0.1_20231023.xlsx
</commit_message>
<xml_diff>
--- a/22KW-Dyno - MCU/Document/MCU TorqueControl CAN协议V0.1_20231023.xlsx
+++ b/22KW-Dyno - MCU/Document/MCU TorqueControl CAN协议V0.1_20231023.xlsx
@@ -2242,6 +2242,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2257,60 +2266,41 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2322,37 +2312,47 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2388,8 +2388,8 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>96</xdr:row>
       <xdr:rowOff>99750</xdr:rowOff>
     </xdr:to>
@@ -2780,13 +2780,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="67" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="17" t="s">
@@ -2795,123 +2795,116 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="65"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
+      <c r="A3" s="68"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
       <c r="D3" s="17" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="65"/>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
+      <c r="A4" s="68"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="17" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="66"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="17" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="63"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
+      <c r="A6" s="66"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
       <c r="E6" s="17"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="63"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
+      <c r="A7" s="66"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
       <c r="D7" s="18"/>
       <c r="E7" s="17"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="63"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="66"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="63"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
       <c r="D9" s="18"/>
       <c r="E9" s="17"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
       <c r="E10" s="17"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="63"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="18"/>
       <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="63"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="66"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="63"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="18"/>
       <c r="E13" s="17"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="63"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="63"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
       <c r="D15" s="18"/>
       <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="63"/>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
+      <c r="A16" s="66"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="66"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="63"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="66"/>
       <c r="D17" s="18"/>
       <c r="E17" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B2:B5"/>
@@ -2926,6 +2919,13 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2937,20 +2937,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.375" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
     <col min="5" max="5" width="3.375" customWidth="1"/>
     <col min="6" max="6" width="2.375" customWidth="1"/>
     <col min="7" max="8" width="2.625" customWidth="1"/>
-    <col min="9" max="9" width="5.375" customWidth="1"/>
-    <col min="10" max="10" width="4.25" customWidth="1"/>
+    <col min="9" max="9" width="3.75" customWidth="1"/>
+    <col min="10" max="10" width="2.75" customWidth="1"/>
     <col min="11" max="22" width="2.625" customWidth="1"/>
+    <col min="23" max="23" width="7.125" customWidth="1"/>
     <col min="24" max="42" width="2.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3088,16 +3089,16 @@
       <c r="D10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="67" t="s">
+      <c r="E10" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="70"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
@@ -3131,26 +3132,26 @@
       <c r="AQ10" s="10"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="83" t="s">
+      <c r="A11" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="84"/>
-      <c r="C11" s="83" t="s">
+      <c r="B11" s="77"/>
+      <c r="C11" s="78" t="s">
         <v>48</v>
       </c>
       <c r="D11" s="85">
         <v>1</v>
       </c>
-      <c r="E11" s="74" t="s">
+      <c r="E11" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="74"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="81"/>
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
@@ -3184,18 +3185,18 @@
       <c r="AQ11" s="11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="83"/>
-      <c r="B12" s="84"/>
-      <c r="C12" s="83"/>
+      <c r="A12" s="78"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
       <c r="D12" s="85"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="74"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="81"/>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
       <c r="O12" s="11"/>
@@ -3229,26 +3230,26 @@
       <c r="AQ12" s="11"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="83" t="s">
+      <c r="A13" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="84"/>
-      <c r="C13" s="83" t="s">
+      <c r="B13" s="77"/>
+      <c r="C13" s="78" t="s">
         <v>48</v>
       </c>
       <c r="D13" s="85">
         <v>1</v>
       </c>
-      <c r="E13" s="74" t="s">
+      <c r="E13" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="74"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
@@ -3282,18 +3283,18 @@
       <c r="AQ13" s="11"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="83"/>
-      <c r="B14" s="84"/>
-      <c r="C14" s="83"/>
+      <c r="A14" s="78"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="78"/>
       <c r="D14" s="85"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="74"/>
-      <c r="J14" s="74"/>
-      <c r="K14" s="74"/>
-      <c r="L14" s="74"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
       <c r="M14" s="11"/>
       <c r="N14" s="11"/>
       <c r="O14" s="11"/>
@@ -3327,26 +3328,26 @@
       <c r="AQ14" s="11"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="89" t="s">
+      <c r="A15" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="84"/>
-      <c r="C15" s="83" t="s">
+      <c r="B15" s="77"/>
+      <c r="C15" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="91">
+      <c r="D15" s="79">
         <v>4</v>
       </c>
-      <c r="E15" s="68" t="s">
+      <c r="E15" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="69"/>
-      <c r="J15" s="69"/>
-      <c r="K15" s="69"/>
-      <c r="L15" s="70"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="94"/>
+      <c r="H15" s="94"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="94"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="95"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
       <c r="O15" s="11"/>
@@ -3380,18 +3381,18 @@
       <c r="AQ15" s="11"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="90"/>
-      <c r="B16" s="84"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="73"/>
+      <c r="A16" s="76"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="97"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="97"/>
+      <c r="K16" s="97"/>
+      <c r="L16" s="98"/>
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
@@ -3425,26 +3426,26 @@
       <c r="AQ16" s="11"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="89" t="s">
+      <c r="A17" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="84"/>
-      <c r="C17" s="83" t="s">
+      <c r="B17" s="77"/>
+      <c r="C17" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="91">
+      <c r="D17" s="79">
         <v>1</v>
       </c>
-      <c r="E17" s="74" t="s">
+      <c r="E17" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="74"/>
-      <c r="K17" s="74"/>
-      <c r="L17" s="74"/>
+      <c r="F17" s="81"/>
+      <c r="G17" s="81"/>
+      <c r="H17" s="81"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="81"/>
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
@@ -3478,18 +3479,18 @@
       <c r="AQ17" s="11"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="90"/>
-      <c r="B18" s="84"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="92"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="74"/>
-      <c r="K18" s="74"/>
-      <c r="L18" s="74"/>
+      <c r="A18" s="76"/>
+      <c r="B18" s="77"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="81"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="81"/>
+      <c r="L18" s="81"/>
       <c r="M18" s="11"/>
       <c r="N18" s="11"/>
       <c r="O18" s="11"/>
@@ -3523,26 +3524,26 @@
       <c r="AQ18" s="11"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="89" t="s">
+      <c r="A19" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="84"/>
-      <c r="C19" s="83" t="s">
+      <c r="B19" s="77"/>
+      <c r="C19" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="91">
+      <c r="D19" s="79">
         <v>1</v>
       </c>
-      <c r="E19" s="74" t="s">
+      <c r="E19" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="74"/>
-      <c r="J19" s="74"/>
-      <c r="K19" s="74"/>
-      <c r="L19" s="74"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81"/>
       <c r="M19" s="11"/>
       <c r="N19" s="11"/>
       <c r="O19" s="11"/>
@@ -3576,18 +3577,18 @@
       <c r="AQ19" s="11"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="90"/>
-      <c r="B20" s="84"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="92"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="74"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
+      <c r="A20" s="76"/>
+      <c r="B20" s="77"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
       <c r="M20" s="11"/>
       <c r="N20" s="11"/>
       <c r="O20" s="11"/>
@@ -3621,26 +3622,26 @@
       <c r="AQ20" s="11"/>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="86" t="s">
+      <c r="A21" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="84"/>
-      <c r="C21" s="86" t="s">
+      <c r="B21" s="77"/>
+      <c r="C21" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="87" t="s">
+      <c r="D21" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="88" t="s">
+      <c r="E21" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="88"/>
-      <c r="G21" s="88"/>
-      <c r="H21" s="88"/>
-      <c r="I21" s="88"/>
-      <c r="J21" s="88"/>
-      <c r="K21" s="88"/>
-      <c r="L21" s="88"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="84"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="84"/>
+      <c r="J21" s="84"/>
+      <c r="K21" s="84"/>
+      <c r="L21" s="84"/>
       <c r="M21" s="12"/>
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
@@ -3674,18 +3675,18 @@
       <c r="AQ21" s="12"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="86"/>
-      <c r="B22" s="84"/>
-      <c r="C22" s="86"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="88"/>
-      <c r="F22" s="88"/>
-      <c r="G22" s="88"/>
-      <c r="H22" s="88"/>
-      <c r="I22" s="88"/>
-      <c r="J22" s="88"/>
-      <c r="K22" s="88"/>
-      <c r="L22" s="88"/>
+      <c r="A22" s="82"/>
+      <c r="B22" s="77"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="83"/>
+      <c r="E22" s="84"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="84"/>
+      <c r="J22" s="84"/>
+      <c r="K22" s="84"/>
+      <c r="L22" s="84"/>
       <c r="M22" s="12"/>
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
@@ -3786,66 +3787,66 @@
       <c r="D29" s="25"/>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A30" s="93" t="s">
+      <c r="A30" s="63" t="s">
         <v>206</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="75" t="s">
+      <c r="C30" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="76"/>
-      <c r="H30" s="76"/>
-      <c r="I30" s="76"/>
-      <c r="J30" s="77"/>
-      <c r="K30" s="75" t="s">
+      <c r="D30" s="90"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="90"/>
+      <c r="J30" s="91"/>
+      <c r="K30" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="L30" s="76"/>
-      <c r="M30" s="76"/>
-      <c r="N30" s="76"/>
-      <c r="O30" s="76"/>
-      <c r="P30" s="76"/>
-      <c r="Q30" s="76"/>
-      <c r="R30" s="77"/>
-      <c r="S30" s="75" t="s">
+      <c r="L30" s="90"/>
+      <c r="M30" s="90"/>
+      <c r="N30" s="90"/>
+      <c r="O30" s="90"/>
+      <c r="P30" s="90"/>
+      <c r="Q30" s="90"/>
+      <c r="R30" s="91"/>
+      <c r="S30" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="T30" s="76"/>
-      <c r="U30" s="76"/>
-      <c r="V30" s="76"/>
-      <c r="W30" s="76"/>
-      <c r="X30" s="76"/>
-      <c r="Y30" s="76"/>
-      <c r="Z30" s="77"/>
-      <c r="AA30" s="75" t="s">
+      <c r="T30" s="90"/>
+      <c r="U30" s="90"/>
+      <c r="V30" s="90"/>
+      <c r="W30" s="90"/>
+      <c r="X30" s="90"/>
+      <c r="Y30" s="90"/>
+      <c r="Z30" s="91"/>
+      <c r="AA30" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="AB30" s="76"/>
-      <c r="AC30" s="76"/>
-      <c r="AD30" s="76"/>
-      <c r="AE30" s="76"/>
-      <c r="AF30" s="76"/>
-      <c r="AG30" s="76"/>
-      <c r="AH30" s="77"/>
-      <c r="AI30" s="75" t="s">
+      <c r="AB30" s="90"/>
+      <c r="AC30" s="90"/>
+      <c r="AD30" s="90"/>
+      <c r="AE30" s="90"/>
+      <c r="AF30" s="90"/>
+      <c r="AG30" s="90"/>
+      <c r="AH30" s="91"/>
+      <c r="AI30" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="AJ30" s="76"/>
-      <c r="AK30" s="76"/>
-      <c r="AL30" s="76"/>
-      <c r="AM30" s="76"/>
-      <c r="AN30" s="76"/>
-      <c r="AO30" s="76"/>
-      <c r="AP30" s="77"/>
+      <c r="AJ30" s="90"/>
+      <c r="AK30" s="90"/>
+      <c r="AL30" s="90"/>
+      <c r="AM30" s="90"/>
+      <c r="AN30" s="90"/>
+      <c r="AO30" s="90"/>
+      <c r="AP30" s="91"/>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
-      <c r="B31" s="94" t="s">
+      <c r="B31" s="71" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="4">
@@ -3971,7 +3972,7 @@
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
-      <c r="B32" s="94"/>
+      <c r="B32" s="71"/>
       <c r="C32" s="52">
         <v>1</v>
       </c>
@@ -4079,57 +4080,57 @@
     </row>
     <row r="33" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A33" s="62"/>
-      <c r="B33" s="94"/>
-      <c r="C33" s="95" t="s">
+      <c r="B33" s="71"/>
+      <c r="C33" s="88" t="s">
         <v>207</v>
       </c>
-      <c r="D33" s="95"/>
-      <c r="E33" s="95"/>
-      <c r="F33" s="95"/>
-      <c r="G33" s="95"/>
-      <c r="H33" s="95"/>
-      <c r="I33" s="95"/>
-      <c r="J33" s="95"/>
-      <c r="K33" s="95" t="s">
+      <c r="D33" s="88"/>
+      <c r="E33" s="88"/>
+      <c r="F33" s="88"/>
+      <c r="G33" s="88"/>
+      <c r="H33" s="88"/>
+      <c r="I33" s="88"/>
+      <c r="J33" s="88"/>
+      <c r="K33" s="88" t="s">
         <v>208</v>
       </c>
-      <c r="L33" s="95"/>
-      <c r="M33" s="95"/>
-      <c r="N33" s="95"/>
-      <c r="O33" s="95"/>
-      <c r="P33" s="95"/>
-      <c r="Q33" s="95"/>
-      <c r="R33" s="95"/>
-      <c r="S33" s="95" t="s">
+      <c r="L33" s="88"/>
+      <c r="M33" s="88"/>
+      <c r="N33" s="88"/>
+      <c r="O33" s="88"/>
+      <c r="P33" s="88"/>
+      <c r="Q33" s="88"/>
+      <c r="R33" s="88"/>
+      <c r="S33" s="88" t="s">
         <v>209</v>
       </c>
-      <c r="T33" s="95"/>
-      <c r="U33" s="95"/>
-      <c r="V33" s="95"/>
-      <c r="W33" s="95"/>
-      <c r="X33" s="95"/>
-      <c r="Y33" s="95"/>
-      <c r="Z33" s="95"/>
-      <c r="AA33" s="95">
+      <c r="T33" s="88"/>
+      <c r="U33" s="88"/>
+      <c r="V33" s="88"/>
+      <c r="W33" s="88"/>
+      <c r="X33" s="88"/>
+      <c r="Y33" s="88"/>
+      <c r="Z33" s="88"/>
+      <c r="AA33" s="88">
         <v>53</v>
       </c>
-      <c r="AB33" s="95"/>
-      <c r="AC33" s="95"/>
-      <c r="AD33" s="95"/>
-      <c r="AE33" s="95"/>
-      <c r="AF33" s="95"/>
-      <c r="AG33" s="95"/>
-      <c r="AH33" s="95"/>
-      <c r="AI33" s="95" t="s">
+      <c r="AB33" s="88"/>
+      <c r="AC33" s="88"/>
+      <c r="AD33" s="88"/>
+      <c r="AE33" s="88"/>
+      <c r="AF33" s="88"/>
+      <c r="AG33" s="88"/>
+      <c r="AH33" s="88"/>
+      <c r="AI33" s="88" t="s">
         <v>210</v>
       </c>
-      <c r="AJ33" s="95"/>
-      <c r="AK33" s="95"/>
-      <c r="AL33" s="95"/>
-      <c r="AM33" s="95"/>
-      <c r="AN33" s="95"/>
-      <c r="AO33" s="95"/>
-      <c r="AP33" s="95"/>
+      <c r="AJ33" s="88"/>
+      <c r="AK33" s="88"/>
+      <c r="AL33" s="88"/>
+      <c r="AM33" s="88"/>
+      <c r="AN33" s="88"/>
+      <c r="AO33" s="88"/>
+      <c r="AP33" s="88"/>
     </row>
     <row r="34" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="27" t="s">
@@ -4185,65 +4186,65 @@
       <c r="AP35" s="2"/>
     </row>
     <row r="36" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A36" s="93" t="s">
+      <c r="A36" s="63" t="s">
         <v>205</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="75" t="s">
+      <c r="C36" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="76"/>
-      <c r="E36" s="76"/>
-      <c r="F36" s="76"/>
-      <c r="G36" s="76"/>
-      <c r="H36" s="76"/>
-      <c r="I36" s="76"/>
-      <c r="J36" s="77"/>
-      <c r="K36" s="75" t="s">
+      <c r="D36" s="90"/>
+      <c r="E36" s="90"/>
+      <c r="F36" s="90"/>
+      <c r="G36" s="90"/>
+      <c r="H36" s="90"/>
+      <c r="I36" s="90"/>
+      <c r="J36" s="91"/>
+      <c r="K36" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="L36" s="76"/>
-      <c r="M36" s="76"/>
-      <c r="N36" s="76"/>
-      <c r="O36" s="76"/>
-      <c r="P36" s="76"/>
-      <c r="Q36" s="76"/>
-      <c r="R36" s="77"/>
-      <c r="S36" s="75" t="s">
+      <c r="L36" s="90"/>
+      <c r="M36" s="90"/>
+      <c r="N36" s="90"/>
+      <c r="O36" s="90"/>
+      <c r="P36" s="90"/>
+      <c r="Q36" s="90"/>
+      <c r="R36" s="91"/>
+      <c r="S36" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="T36" s="76"/>
-      <c r="U36" s="76"/>
-      <c r="V36" s="76"/>
-      <c r="W36" s="76"/>
-      <c r="X36" s="76"/>
-      <c r="Y36" s="76"/>
-      <c r="Z36" s="77"/>
-      <c r="AA36" s="75" t="s">
+      <c r="T36" s="90"/>
+      <c r="U36" s="90"/>
+      <c r="V36" s="90"/>
+      <c r="W36" s="90"/>
+      <c r="X36" s="90"/>
+      <c r="Y36" s="90"/>
+      <c r="Z36" s="91"/>
+      <c r="AA36" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="AB36" s="76"/>
-      <c r="AC36" s="76"/>
-      <c r="AD36" s="76"/>
-      <c r="AE36" s="76"/>
-      <c r="AF36" s="76"/>
-      <c r="AG36" s="76"/>
-      <c r="AH36" s="77"/>
-      <c r="AI36" s="75" t="s">
+      <c r="AB36" s="90"/>
+      <c r="AC36" s="90"/>
+      <c r="AD36" s="90"/>
+      <c r="AE36" s="90"/>
+      <c r="AF36" s="90"/>
+      <c r="AG36" s="90"/>
+      <c r="AH36" s="91"/>
+      <c r="AI36" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="AJ36" s="76"/>
-      <c r="AK36" s="76"/>
-      <c r="AL36" s="76"/>
-      <c r="AM36" s="76"/>
-      <c r="AN36" s="76"/>
-      <c r="AO36" s="76"/>
-      <c r="AP36" s="77"/>
+      <c r="AJ36" s="90"/>
+      <c r="AK36" s="90"/>
+      <c r="AL36" s="90"/>
+      <c r="AM36" s="90"/>
+      <c r="AN36" s="90"/>
+      <c r="AO36" s="90"/>
+      <c r="AP36" s="91"/>
     </row>
     <row r="37" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="B37" s="80" t="s">
+      <c r="B37" s="72" t="s">
         <v>19</v>
       </c>
       <c r="C37" s="4">
@@ -4369,7 +4370,7 @@
     </row>
     <row r="38" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
-      <c r="B38" s="97"/>
+      <c r="B38" s="73"/>
       <c r="C38" s="52">
         <v>1</v>
       </c>
@@ -4477,57 +4478,57 @@
     </row>
     <row r="39" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A39" s="62"/>
-      <c r="B39" s="81"/>
-      <c r="C39" s="67" t="s">
+      <c r="B39" s="74"/>
+      <c r="C39" s="70" t="s">
         <v>211</v>
       </c>
-      <c r="D39" s="67"/>
-      <c r="E39" s="67"/>
-      <c r="F39" s="67"/>
-      <c r="G39" s="67"/>
-      <c r="H39" s="67"/>
-      <c r="I39" s="67"/>
-      <c r="J39" s="67"/>
-      <c r="K39" s="67" t="s">
+      <c r="D39" s="70"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="70"/>
+      <c r="J39" s="70"/>
+      <c r="K39" s="70" t="s">
         <v>208</v>
       </c>
-      <c r="L39" s="67"/>
-      <c r="M39" s="67"/>
-      <c r="N39" s="67"/>
-      <c r="O39" s="67"/>
-      <c r="P39" s="67"/>
-      <c r="Q39" s="67"/>
-      <c r="R39" s="67"/>
-      <c r="S39" s="67" t="s">
+      <c r="L39" s="70"/>
+      <c r="M39" s="70"/>
+      <c r="N39" s="70"/>
+      <c r="O39" s="70"/>
+      <c r="P39" s="70"/>
+      <c r="Q39" s="70"/>
+      <c r="R39" s="70"/>
+      <c r="S39" s="70" t="s">
         <v>212</v>
       </c>
-      <c r="T39" s="67"/>
-      <c r="U39" s="67"/>
-      <c r="V39" s="67"/>
-      <c r="W39" s="67"/>
-      <c r="X39" s="67"/>
-      <c r="Y39" s="67"/>
-      <c r="Z39" s="67"/>
-      <c r="AA39" s="67">
+      <c r="T39" s="70"/>
+      <c r="U39" s="70"/>
+      <c r="V39" s="70"/>
+      <c r="W39" s="70"/>
+      <c r="X39" s="70"/>
+      <c r="Y39" s="70"/>
+      <c r="Z39" s="70"/>
+      <c r="AA39" s="70">
         <v>53</v>
       </c>
-      <c r="AB39" s="67"/>
-      <c r="AC39" s="67"/>
-      <c r="AD39" s="67"/>
-      <c r="AE39" s="67"/>
-      <c r="AF39" s="67"/>
-      <c r="AG39" s="67"/>
-      <c r="AH39" s="67"/>
-      <c r="AI39" s="67" t="s">
+      <c r="AB39" s="70"/>
+      <c r="AC39" s="70"/>
+      <c r="AD39" s="70"/>
+      <c r="AE39" s="70"/>
+      <c r="AF39" s="70"/>
+      <c r="AG39" s="70"/>
+      <c r="AH39" s="70"/>
+      <c r="AI39" s="70" t="s">
         <v>213</v>
       </c>
-      <c r="AJ39" s="67"/>
-      <c r="AK39" s="67"/>
-      <c r="AL39" s="67"/>
-      <c r="AM39" s="67"/>
-      <c r="AN39" s="67"/>
-      <c r="AO39" s="67"/>
-      <c r="AP39" s="67"/>
+      <c r="AJ39" s="70"/>
+      <c r="AK39" s="70"/>
+      <c r="AL39" s="70"/>
+      <c r="AM39" s="70"/>
+      <c r="AN39" s="70"/>
+      <c r="AO39" s="70"/>
+      <c r="AP39" s="70"/>
     </row>
     <row r="40" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="27" t="s">
@@ -4555,17 +4556,17 @@
       <c r="U40" s="6"/>
       <c r="V40" s="6"/>
       <c r="W40" s="6"/>
-      <c r="X40" s="96"/>
-      <c r="Y40" s="96"/>
-      <c r="Z40" s="96"/>
-      <c r="AA40" s="96"/>
-      <c r="AB40" s="96"/>
-      <c r="AC40" s="96"/>
-      <c r="AD40" s="96"/>
-      <c r="AE40" s="96"/>
-      <c r="AF40" s="96"/>
-      <c r="AG40" s="96"/>
-      <c r="AH40" s="96"/>
+      <c r="X40" s="64"/>
+      <c r="Y40" s="64"/>
+      <c r="Z40" s="64"/>
+      <c r="AA40" s="64"/>
+      <c r="AB40" s="64"/>
+      <c r="AC40" s="64"/>
+      <c r="AD40" s="64"/>
+      <c r="AE40" s="64"/>
+      <c r="AF40" s="64"/>
+      <c r="AG40" s="64"/>
+      <c r="AH40" s="64"/>
       <c r="AI40" s="6"/>
       <c r="AJ40" s="6"/>
       <c r="AK40" s="6"/>
@@ -4603,19 +4604,19 @@
       <c r="W41" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="X41" s="82" t="s">
+      <c r="X41" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="Y41" s="82"/>
-      <c r="Z41" s="82"/>
-      <c r="AA41" s="82"/>
-      <c r="AB41" s="82"/>
-      <c r="AC41" s="82"/>
-      <c r="AD41" s="82"/>
-      <c r="AE41" s="82"/>
-      <c r="AF41" s="82"/>
-      <c r="AG41" s="82"/>
-      <c r="AH41" s="82"/>
+      <c r="Y41" s="87"/>
+      <c r="Z41" s="87"/>
+      <c r="AA41" s="87"/>
+      <c r="AB41" s="87"/>
+      <c r="AC41" s="87"/>
+      <c r="AD41" s="87"/>
+      <c r="AE41" s="87"/>
+      <c r="AF41" s="87"/>
+      <c r="AG41" s="87"/>
+      <c r="AH41" s="87"/>
       <c r="AI41" s="2"/>
       <c r="AJ41" s="2"/>
       <c r="AK41" s="2"/>
@@ -4626,66 +4627,66 @@
       <c r="AP41" s="2"/>
     </row>
     <row r="42" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A42" s="93" t="s">
+      <c r="A42" s="63" t="s">
         <v>203</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="75" t="s">
+      <c r="C42" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="76"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="76"/>
-      <c r="G42" s="76"/>
-      <c r="H42" s="76"/>
-      <c r="I42" s="76"/>
-      <c r="J42" s="77"/>
-      <c r="K42" s="75" t="s">
+      <c r="D42" s="90"/>
+      <c r="E42" s="90"/>
+      <c r="F42" s="90"/>
+      <c r="G42" s="90"/>
+      <c r="H42" s="90"/>
+      <c r="I42" s="90"/>
+      <c r="J42" s="91"/>
+      <c r="K42" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="L42" s="76"/>
-      <c r="M42" s="76"/>
-      <c r="N42" s="76"/>
-      <c r="O42" s="76"/>
-      <c r="P42" s="76"/>
-      <c r="Q42" s="76"/>
-      <c r="R42" s="77"/>
-      <c r="S42" s="75" t="s">
+      <c r="L42" s="90"/>
+      <c r="M42" s="90"/>
+      <c r="N42" s="90"/>
+      <c r="O42" s="90"/>
+      <c r="P42" s="90"/>
+      <c r="Q42" s="90"/>
+      <c r="R42" s="91"/>
+      <c r="S42" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="T42" s="76"/>
-      <c r="U42" s="76"/>
-      <c r="V42" s="76"/>
-      <c r="W42" s="76"/>
-      <c r="X42" s="76"/>
-      <c r="Y42" s="76"/>
-      <c r="Z42" s="77"/>
-      <c r="AA42" s="75" t="s">
+      <c r="T42" s="90"/>
+      <c r="U42" s="90"/>
+      <c r="V42" s="90"/>
+      <c r="W42" s="90"/>
+      <c r="X42" s="90"/>
+      <c r="Y42" s="90"/>
+      <c r="Z42" s="91"/>
+      <c r="AA42" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="AB42" s="76"/>
-      <c r="AC42" s="76"/>
-      <c r="AD42" s="76"/>
-      <c r="AE42" s="76"/>
-      <c r="AF42" s="76"/>
-      <c r="AG42" s="76"/>
-      <c r="AH42" s="77"/>
-      <c r="AI42" s="75" t="s">
+      <c r="AB42" s="90"/>
+      <c r="AC42" s="90"/>
+      <c r="AD42" s="90"/>
+      <c r="AE42" s="90"/>
+      <c r="AF42" s="90"/>
+      <c r="AG42" s="90"/>
+      <c r="AH42" s="91"/>
+      <c r="AI42" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="AJ42" s="76"/>
-      <c r="AK42" s="76"/>
-      <c r="AL42" s="76"/>
-      <c r="AM42" s="76"/>
-      <c r="AN42" s="76"/>
-      <c r="AO42" s="76"/>
-      <c r="AP42" s="77"/>
+      <c r="AJ42" s="90"/>
+      <c r="AK42" s="90"/>
+      <c r="AL42" s="90"/>
+      <c r="AM42" s="90"/>
+      <c r="AN42" s="90"/>
+      <c r="AO42" s="90"/>
+      <c r="AP42" s="91"/>
     </row>
     <row r="43" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
-      <c r="B43" s="80" t="s">
+      <c r="B43" s="72" t="s">
         <v>19</v>
       </c>
       <c r="C43" s="4">
@@ -4811,7 +4812,7 @@
     </row>
     <row r="44" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
-      <c r="B44" s="97"/>
+      <c r="B44" s="73"/>
       <c r="C44" s="52">
         <v>1</v>
       </c>
@@ -4872,7 +4873,7 @@
       <c r="V44" s="14">
         <v>0</v>
       </c>
-      <c r="W44" s="98">
+      <c r="W44" s="65">
         <v>1</v>
       </c>
       <c r="X44" s="60">
@@ -4919,57 +4920,57 @@
     </row>
     <row r="45" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A45" s="62"/>
-      <c r="B45" s="81"/>
-      <c r="C45" s="67" t="s">
+      <c r="B45" s="74"/>
+      <c r="C45" s="70" t="s">
         <v>211</v>
       </c>
-      <c r="D45" s="67"/>
-      <c r="E45" s="67"/>
-      <c r="F45" s="67"/>
-      <c r="G45" s="67"/>
-      <c r="H45" s="67"/>
-      <c r="I45" s="67"/>
-      <c r="J45" s="67"/>
-      <c r="K45" s="67" t="s">
+      <c r="D45" s="70"/>
+      <c r="E45" s="70"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="70"/>
+      <c r="H45" s="70"/>
+      <c r="I45" s="70"/>
+      <c r="J45" s="70"/>
+      <c r="K45" s="70" t="s">
         <v>208</v>
       </c>
-      <c r="L45" s="67"/>
-      <c r="M45" s="67"/>
-      <c r="N45" s="67"/>
-      <c r="O45" s="67"/>
-      <c r="P45" s="67"/>
-      <c r="Q45" s="67"/>
-      <c r="R45" s="67"/>
-      <c r="S45" s="67" t="s">
+      <c r="L45" s="70"/>
+      <c r="M45" s="70"/>
+      <c r="N45" s="70"/>
+      <c r="O45" s="70"/>
+      <c r="P45" s="70"/>
+      <c r="Q45" s="70"/>
+      <c r="R45" s="70"/>
+      <c r="S45" s="70" t="s">
         <v>214</v>
       </c>
-      <c r="T45" s="67"/>
-      <c r="U45" s="67"/>
-      <c r="V45" s="67"/>
-      <c r="W45" s="67"/>
-      <c r="X45" s="67"/>
-      <c r="Y45" s="67"/>
-      <c r="Z45" s="67"/>
-      <c r="AA45" s="67">
+      <c r="T45" s="70"/>
+      <c r="U45" s="70"/>
+      <c r="V45" s="70"/>
+      <c r="W45" s="70"/>
+      <c r="X45" s="70"/>
+      <c r="Y45" s="70"/>
+      <c r="Z45" s="70"/>
+      <c r="AA45" s="70">
         <v>53</v>
       </c>
-      <c r="AB45" s="67"/>
-      <c r="AC45" s="67"/>
-      <c r="AD45" s="67"/>
-      <c r="AE45" s="67"/>
-      <c r="AF45" s="67"/>
-      <c r="AG45" s="67"/>
-      <c r="AH45" s="67"/>
-      <c r="AI45" s="67" t="s">
+      <c r="AB45" s="70"/>
+      <c r="AC45" s="70"/>
+      <c r="AD45" s="70"/>
+      <c r="AE45" s="70"/>
+      <c r="AF45" s="70"/>
+      <c r="AG45" s="70"/>
+      <c r="AH45" s="70"/>
+      <c r="AI45" s="70" t="s">
         <v>213</v>
       </c>
-      <c r="AJ45" s="67"/>
-      <c r="AK45" s="67"/>
-      <c r="AL45" s="67"/>
-      <c r="AM45" s="67"/>
-      <c r="AN45" s="67"/>
-      <c r="AO45" s="67"/>
-      <c r="AP45" s="67"/>
+      <c r="AJ45" s="70"/>
+      <c r="AK45" s="70"/>
+      <c r="AL45" s="70"/>
+      <c r="AM45" s="70"/>
+      <c r="AN45" s="70"/>
+      <c r="AO45" s="70"/>
+      <c r="AP45" s="70"/>
     </row>
     <row r="46" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="27" t="s">
@@ -5025,68 +5026,68 @@
       <c r="AP47" s="2"/>
     </row>
     <row r="48" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A48" s="93" t="s">
+      <c r="A48" s="63" t="s">
         <v>204</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C48" s="78" t="s">
+      <c r="C48" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="78"/>
-      <c r="E48" s="78"/>
-      <c r="F48" s="78"/>
-      <c r="G48" s="78"/>
-      <c r="H48" s="78"/>
-      <c r="I48" s="78"/>
-      <c r="J48" s="78"/>
-      <c r="K48" s="78" t="s">
+      <c r="D48" s="92"/>
+      <c r="E48" s="92"/>
+      <c r="F48" s="92"/>
+      <c r="G48" s="92"/>
+      <c r="H48" s="92"/>
+      <c r="I48" s="92"/>
+      <c r="J48" s="92"/>
+      <c r="K48" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="L48" s="78"/>
-      <c r="M48" s="78"/>
-      <c r="N48" s="78"/>
-      <c r="O48" s="78"/>
-      <c r="P48" s="78"/>
-      <c r="Q48" s="78"/>
-      <c r="R48" s="78"/>
-      <c r="S48" s="78" t="s">
+      <c r="L48" s="92"/>
+      <c r="M48" s="92"/>
+      <c r="N48" s="92"/>
+      <c r="O48" s="92"/>
+      <c r="P48" s="92"/>
+      <c r="Q48" s="92"/>
+      <c r="R48" s="92"/>
+      <c r="S48" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="T48" s="78"/>
-      <c r="U48" s="78"/>
-      <c r="V48" s="78"/>
-      <c r="W48" s="78"/>
-      <c r="X48" s="78"/>
-      <c r="Y48" s="78"/>
-      <c r="Z48" s="78"/>
-      <c r="AA48" s="78" t="s">
+      <c r="T48" s="92"/>
+      <c r="U48" s="92"/>
+      <c r="V48" s="92"/>
+      <c r="W48" s="92"/>
+      <c r="X48" s="92"/>
+      <c r="Y48" s="92"/>
+      <c r="Z48" s="92"/>
+      <c r="AA48" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="AB48" s="78"/>
-      <c r="AC48" s="78"/>
-      <c r="AD48" s="78"/>
-      <c r="AE48" s="78"/>
-      <c r="AF48" s="78"/>
-      <c r="AG48" s="78"/>
-      <c r="AH48" s="78"/>
-      <c r="AI48" s="78" t="s">
+      <c r="AB48" s="92"/>
+      <c r="AC48" s="92"/>
+      <c r="AD48" s="92"/>
+      <c r="AE48" s="92"/>
+      <c r="AF48" s="92"/>
+      <c r="AG48" s="92"/>
+      <c r="AH48" s="92"/>
+      <c r="AI48" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="AJ48" s="78"/>
-      <c r="AK48" s="78"/>
-      <c r="AL48" s="78"/>
-      <c r="AM48" s="78"/>
-      <c r="AN48" s="78"/>
-      <c r="AO48" s="78"/>
-      <c r="AP48" s="78"/>
+      <c r="AJ48" s="92"/>
+      <c r="AK48" s="92"/>
+      <c r="AL48" s="92"/>
+      <c r="AM48" s="92"/>
+      <c r="AN48" s="92"/>
+      <c r="AO48" s="92"/>
+      <c r="AP48" s="92"/>
     </row>
     <row r="49" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B49" s="94" t="s">
+      <c r="B49" s="71" t="s">
         <v>19</v>
       </c>
       <c r="C49" s="4">
@@ -5212,7 +5213,7 @@
     </row>
     <row r="50" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
-      <c r="B50" s="94"/>
+      <c r="B50" s="71"/>
       <c r="C50" s="52">
         <v>1</v>
       </c>
@@ -5320,57 +5321,57 @@
     </row>
     <row r="51" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A51" s="62"/>
-      <c r="B51" s="94"/>
-      <c r="C51" s="67" t="s">
+      <c r="B51" s="71"/>
+      <c r="C51" s="70" t="s">
         <v>211</v>
       </c>
-      <c r="D51" s="67"/>
-      <c r="E51" s="67"/>
-      <c r="F51" s="67"/>
-      <c r="G51" s="67"/>
-      <c r="H51" s="67"/>
-      <c r="I51" s="67"/>
-      <c r="J51" s="67"/>
-      <c r="K51" s="67" t="s">
+      <c r="D51" s="70"/>
+      <c r="E51" s="70"/>
+      <c r="F51" s="70"/>
+      <c r="G51" s="70"/>
+      <c r="H51" s="70"/>
+      <c r="I51" s="70"/>
+      <c r="J51" s="70"/>
+      <c r="K51" s="70" t="s">
         <v>208</v>
       </c>
-      <c r="L51" s="67"/>
-      <c r="M51" s="67"/>
-      <c r="N51" s="67"/>
-      <c r="O51" s="67"/>
-      <c r="P51" s="67"/>
-      <c r="Q51" s="67"/>
-      <c r="R51" s="67"/>
-      <c r="S51" s="67" t="s">
+      <c r="L51" s="70"/>
+      <c r="M51" s="70"/>
+      <c r="N51" s="70"/>
+      <c r="O51" s="70"/>
+      <c r="P51" s="70"/>
+      <c r="Q51" s="70"/>
+      <c r="R51" s="70"/>
+      <c r="S51" s="70" t="s">
         <v>215</v>
       </c>
-      <c r="T51" s="67"/>
-      <c r="U51" s="67"/>
-      <c r="V51" s="67"/>
-      <c r="W51" s="67"/>
-      <c r="X51" s="67"/>
-      <c r="Y51" s="67"/>
-      <c r="Z51" s="67"/>
-      <c r="AA51" s="67">
+      <c r="T51" s="70"/>
+      <c r="U51" s="70"/>
+      <c r="V51" s="70"/>
+      <c r="W51" s="70"/>
+      <c r="X51" s="70"/>
+      <c r="Y51" s="70"/>
+      <c r="Z51" s="70"/>
+      <c r="AA51" s="70">
         <v>53</v>
       </c>
-      <c r="AB51" s="67"/>
-      <c r="AC51" s="67"/>
-      <c r="AD51" s="67"/>
-      <c r="AE51" s="67"/>
-      <c r="AF51" s="67"/>
-      <c r="AG51" s="67"/>
-      <c r="AH51" s="67"/>
-      <c r="AI51" s="67" t="s">
+      <c r="AB51" s="70"/>
+      <c r="AC51" s="70"/>
+      <c r="AD51" s="70"/>
+      <c r="AE51" s="70"/>
+      <c r="AF51" s="70"/>
+      <c r="AG51" s="70"/>
+      <c r="AH51" s="70"/>
+      <c r="AI51" s="70" t="s">
         <v>213</v>
       </c>
-      <c r="AJ51" s="67"/>
-      <c r="AK51" s="67"/>
-      <c r="AL51" s="67"/>
-      <c r="AM51" s="67"/>
-      <c r="AN51" s="67"/>
-      <c r="AO51" s="67"/>
-      <c r="AP51" s="67"/>
+      <c r="AJ51" s="70"/>
+      <c r="AK51" s="70"/>
+      <c r="AL51" s="70"/>
+      <c r="AM51" s="70"/>
+      <c r="AN51" s="70"/>
+      <c r="AO51" s="70"/>
+      <c r="AP51" s="70"/>
     </row>
     <row r="52" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="27" t="s">
@@ -5446,19 +5447,19 @@
       <c r="W53" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="X53" s="79" t="s">
+      <c r="X53" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="Y53" s="79"/>
-      <c r="Z53" s="79"/>
-      <c r="AA53" s="79"/>
-      <c r="AB53" s="79"/>
-      <c r="AC53" s="79"/>
-      <c r="AD53" s="79"/>
-      <c r="AE53" s="79"/>
-      <c r="AF53" s="79"/>
-      <c r="AG53" s="79"/>
-      <c r="AH53" s="79"/>
+      <c r="Y53" s="86"/>
+      <c r="Z53" s="86"/>
+      <c r="AA53" s="86"/>
+      <c r="AB53" s="86"/>
+      <c r="AC53" s="86"/>
+      <c r="AD53" s="86"/>
+      <c r="AE53" s="86"/>
+      <c r="AF53" s="86"/>
+      <c r="AG53" s="86"/>
+      <c r="AH53" s="86"/>
       <c r="AI53" s="2"/>
       <c r="AJ53" s="2"/>
       <c r="AK53" s="2"/>
@@ -5469,66 +5470,66 @@
       <c r="AP53" s="2"/>
     </row>
     <row r="54" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A54" s="93" t="s">
+      <c r="A54" s="63" t="s">
         <v>203</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C54" s="75" t="s">
+      <c r="C54" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="D54" s="76"/>
-      <c r="E54" s="76"/>
-      <c r="F54" s="76"/>
-      <c r="G54" s="76"/>
-      <c r="H54" s="76"/>
-      <c r="I54" s="76"/>
-      <c r="J54" s="77"/>
-      <c r="K54" s="75" t="s">
+      <c r="D54" s="90"/>
+      <c r="E54" s="90"/>
+      <c r="F54" s="90"/>
+      <c r="G54" s="90"/>
+      <c r="H54" s="90"/>
+      <c r="I54" s="90"/>
+      <c r="J54" s="91"/>
+      <c r="K54" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="L54" s="76"/>
-      <c r="M54" s="76"/>
-      <c r="N54" s="76"/>
-      <c r="O54" s="76"/>
-      <c r="P54" s="76"/>
-      <c r="Q54" s="76"/>
-      <c r="R54" s="77"/>
-      <c r="S54" s="75" t="s">
+      <c r="L54" s="90"/>
+      <c r="M54" s="90"/>
+      <c r="N54" s="90"/>
+      <c r="O54" s="90"/>
+      <c r="P54" s="90"/>
+      <c r="Q54" s="90"/>
+      <c r="R54" s="91"/>
+      <c r="S54" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="T54" s="76"/>
-      <c r="U54" s="76"/>
-      <c r="V54" s="76"/>
-      <c r="W54" s="76"/>
-      <c r="X54" s="76"/>
-      <c r="Y54" s="76"/>
-      <c r="Z54" s="77"/>
-      <c r="AA54" s="75" t="s">
+      <c r="T54" s="90"/>
+      <c r="U54" s="90"/>
+      <c r="V54" s="90"/>
+      <c r="W54" s="90"/>
+      <c r="X54" s="90"/>
+      <c r="Y54" s="90"/>
+      <c r="Z54" s="91"/>
+      <c r="AA54" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="AB54" s="76"/>
-      <c r="AC54" s="76"/>
-      <c r="AD54" s="76"/>
-      <c r="AE54" s="76"/>
-      <c r="AF54" s="76"/>
-      <c r="AG54" s="76"/>
-      <c r="AH54" s="77"/>
-      <c r="AI54" s="75" t="s">
+      <c r="AB54" s="90"/>
+      <c r="AC54" s="90"/>
+      <c r="AD54" s="90"/>
+      <c r="AE54" s="90"/>
+      <c r="AF54" s="90"/>
+      <c r="AG54" s="90"/>
+      <c r="AH54" s="91"/>
+      <c r="AI54" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="AJ54" s="76"/>
-      <c r="AK54" s="76"/>
-      <c r="AL54" s="76"/>
-      <c r="AM54" s="76"/>
-      <c r="AN54" s="76"/>
-      <c r="AO54" s="76"/>
-      <c r="AP54" s="77"/>
+      <c r="AJ54" s="90"/>
+      <c r="AK54" s="90"/>
+      <c r="AL54" s="90"/>
+      <c r="AM54" s="90"/>
+      <c r="AN54" s="90"/>
+      <c r="AO54" s="90"/>
+      <c r="AP54" s="91"/>
     </row>
     <row r="55" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
-      <c r="B55" s="80" t="s">
+      <c r="B55" s="72" t="s">
         <v>19</v>
       </c>
       <c r="C55" s="4">
@@ -5654,7 +5655,7 @@
     </row>
     <row r="56" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
-      <c r="B56" s="97"/>
+      <c r="B56" s="73"/>
       <c r="C56" s="52">
         <v>1</v>
       </c>
@@ -5715,7 +5716,7 @@
       <c r="V56" s="14">
         <v>0</v>
       </c>
-      <c r="W56" s="98">
+      <c r="W56" s="65">
         <v>1</v>
       </c>
       <c r="X56" s="60">
@@ -5762,57 +5763,57 @@
     </row>
     <row r="57" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A57" s="62"/>
-      <c r="B57" s="81"/>
-      <c r="C57" s="67" t="s">
+      <c r="B57" s="74"/>
+      <c r="C57" s="70" t="s">
         <v>211</v>
       </c>
-      <c r="D57" s="67"/>
-      <c r="E57" s="67"/>
-      <c r="F57" s="67"/>
-      <c r="G57" s="67"/>
-      <c r="H57" s="67"/>
-      <c r="I57" s="67"/>
-      <c r="J57" s="67"/>
-      <c r="K57" s="67" t="s">
+      <c r="D57" s="70"/>
+      <c r="E57" s="70"/>
+      <c r="F57" s="70"/>
+      <c r="G57" s="70"/>
+      <c r="H57" s="70"/>
+      <c r="I57" s="70"/>
+      <c r="J57" s="70"/>
+      <c r="K57" s="70" t="s">
         <v>208</v>
       </c>
-      <c r="L57" s="67"/>
-      <c r="M57" s="67"/>
-      <c r="N57" s="67"/>
-      <c r="O57" s="67"/>
-      <c r="P57" s="67"/>
-      <c r="Q57" s="67"/>
-      <c r="R57" s="67"/>
-      <c r="S57" s="67" t="s">
+      <c r="L57" s="70"/>
+      <c r="M57" s="70"/>
+      <c r="N57" s="70"/>
+      <c r="O57" s="70"/>
+      <c r="P57" s="70"/>
+      <c r="Q57" s="70"/>
+      <c r="R57" s="70"/>
+      <c r="S57" s="70" t="s">
         <v>214</v>
       </c>
-      <c r="T57" s="67"/>
-      <c r="U57" s="67"/>
-      <c r="V57" s="67"/>
-      <c r="W57" s="67"/>
-      <c r="X57" s="67"/>
-      <c r="Y57" s="67"/>
-      <c r="Z57" s="67"/>
-      <c r="AA57" s="67">
+      <c r="T57" s="70"/>
+      <c r="U57" s="70"/>
+      <c r="V57" s="70"/>
+      <c r="W57" s="70"/>
+      <c r="X57" s="70"/>
+      <c r="Y57" s="70"/>
+      <c r="Z57" s="70"/>
+      <c r="AA57" s="70">
         <v>53</v>
       </c>
-      <c r="AB57" s="67"/>
-      <c r="AC57" s="67"/>
-      <c r="AD57" s="67"/>
-      <c r="AE57" s="67"/>
-      <c r="AF57" s="67"/>
-      <c r="AG57" s="67"/>
-      <c r="AH57" s="67"/>
-      <c r="AI57" s="67" t="s">
+      <c r="AB57" s="70"/>
+      <c r="AC57" s="70"/>
+      <c r="AD57" s="70"/>
+      <c r="AE57" s="70"/>
+      <c r="AF57" s="70"/>
+      <c r="AG57" s="70"/>
+      <c r="AH57" s="70"/>
+      <c r="AI57" s="70" t="s">
         <v>213</v>
       </c>
-      <c r="AJ57" s="67"/>
-      <c r="AK57" s="67"/>
-      <c r="AL57" s="67"/>
-      <c r="AM57" s="67"/>
-      <c r="AN57" s="67"/>
-      <c r="AO57" s="67"/>
-      <c r="AP57" s="67"/>
+      <c r="AJ57" s="70"/>
+      <c r="AK57" s="70"/>
+      <c r="AL57" s="70"/>
+      <c r="AM57" s="70"/>
+      <c r="AN57" s="70"/>
+      <c r="AO57" s="70"/>
+      <c r="AP57" s="70"/>
     </row>
     <row r="58" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="27" t="s">
@@ -5866,66 +5867,66 @@
       <c r="AP59" s="2"/>
     </row>
     <row r="60" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A60" s="93" t="s">
+      <c r="A60" s="63" t="s">
         <v>206</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C60" s="78" t="s">
+      <c r="C60" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="D60" s="78"/>
-      <c r="E60" s="78"/>
-      <c r="F60" s="78"/>
-      <c r="G60" s="78"/>
-      <c r="H60" s="78"/>
-      <c r="I60" s="78"/>
-      <c r="J60" s="78"/>
-      <c r="K60" s="78" t="s">
+      <c r="D60" s="92"/>
+      <c r="E60" s="92"/>
+      <c r="F60" s="92"/>
+      <c r="G60" s="92"/>
+      <c r="H60" s="92"/>
+      <c r="I60" s="92"/>
+      <c r="J60" s="92"/>
+      <c r="K60" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="L60" s="78"/>
-      <c r="M60" s="78"/>
-      <c r="N60" s="78"/>
-      <c r="O60" s="78"/>
-      <c r="P60" s="78"/>
-      <c r="Q60" s="78"/>
-      <c r="R60" s="78"/>
-      <c r="S60" s="78" t="s">
+      <c r="L60" s="92"/>
+      <c r="M60" s="92"/>
+      <c r="N60" s="92"/>
+      <c r="O60" s="92"/>
+      <c r="P60" s="92"/>
+      <c r="Q60" s="92"/>
+      <c r="R60" s="92"/>
+      <c r="S60" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="T60" s="78"/>
-      <c r="U60" s="78"/>
-      <c r="V60" s="78"/>
-      <c r="W60" s="78"/>
-      <c r="X60" s="78"/>
-      <c r="Y60" s="78"/>
-      <c r="Z60" s="78"/>
-      <c r="AA60" s="78" t="s">
+      <c r="T60" s="92"/>
+      <c r="U60" s="92"/>
+      <c r="V60" s="92"/>
+      <c r="W60" s="92"/>
+      <c r="X60" s="92"/>
+      <c r="Y60" s="92"/>
+      <c r="Z60" s="92"/>
+      <c r="AA60" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="AB60" s="78"/>
-      <c r="AC60" s="78"/>
-      <c r="AD60" s="78"/>
-      <c r="AE60" s="78"/>
-      <c r="AF60" s="78"/>
-      <c r="AG60" s="78"/>
-      <c r="AH60" s="78"/>
-      <c r="AI60" s="78" t="s">
+      <c r="AB60" s="92"/>
+      <c r="AC60" s="92"/>
+      <c r="AD60" s="92"/>
+      <c r="AE60" s="92"/>
+      <c r="AF60" s="92"/>
+      <c r="AG60" s="92"/>
+      <c r="AH60" s="92"/>
+      <c r="AI60" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="AJ60" s="78"/>
-      <c r="AK60" s="78"/>
-      <c r="AL60" s="78"/>
-      <c r="AM60" s="78"/>
-      <c r="AN60" s="78"/>
-      <c r="AO60" s="78"/>
-      <c r="AP60" s="78"/>
+      <c r="AJ60" s="92"/>
+      <c r="AK60" s="92"/>
+      <c r="AL60" s="92"/>
+      <c r="AM60" s="92"/>
+      <c r="AN60" s="92"/>
+      <c r="AO60" s="92"/>
+      <c r="AP60" s="92"/>
     </row>
     <row r="61" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
-      <c r="B61" s="94" t="s">
+      <c r="B61" s="71" t="s">
         <v>19</v>
       </c>
       <c r="C61" s="4">
@@ -6051,7 +6052,7 @@
     </row>
     <row r="62" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
-      <c r="B62" s="94"/>
+      <c r="B62" s="71"/>
       <c r="C62" s="4">
         <v>0</v>
       </c>
@@ -6159,145 +6160,60 @@
     </row>
     <row r="63" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
-      <c r="B63" s="94"/>
-      <c r="C63" s="67" t="s">
+      <c r="B63" s="71"/>
+      <c r="C63" s="70" t="s">
         <v>211</v>
       </c>
-      <c r="D63" s="67"/>
-      <c r="E63" s="67"/>
-      <c r="F63" s="67"/>
-      <c r="G63" s="67"/>
-      <c r="H63" s="67"/>
-      <c r="I63" s="67"/>
-      <c r="J63" s="67"/>
-      <c r="K63" s="67" t="s">
+      <c r="D63" s="70"/>
+      <c r="E63" s="70"/>
+      <c r="F63" s="70"/>
+      <c r="G63" s="70"/>
+      <c r="H63" s="70"/>
+      <c r="I63" s="70"/>
+      <c r="J63" s="70"/>
+      <c r="K63" s="70" t="s">
         <v>208</v>
       </c>
-      <c r="L63" s="67"/>
-      <c r="M63" s="67"/>
-      <c r="N63" s="67"/>
-      <c r="O63" s="67"/>
-      <c r="P63" s="67"/>
-      <c r="Q63" s="67"/>
-      <c r="R63" s="67"/>
-      <c r="S63" s="67" t="s">
+      <c r="L63" s="70"/>
+      <c r="M63" s="70"/>
+      <c r="N63" s="70"/>
+      <c r="O63" s="70"/>
+      <c r="P63" s="70"/>
+      <c r="Q63" s="70"/>
+      <c r="R63" s="70"/>
+      <c r="S63" s="70" t="s">
         <v>212</v>
       </c>
-      <c r="T63" s="67"/>
-      <c r="U63" s="67"/>
-      <c r="V63" s="67"/>
-      <c r="W63" s="67"/>
-      <c r="X63" s="67"/>
-      <c r="Y63" s="67"/>
-      <c r="Z63" s="67"/>
-      <c r="AA63" s="67">
+      <c r="T63" s="70"/>
+      <c r="U63" s="70"/>
+      <c r="V63" s="70"/>
+      <c r="W63" s="70"/>
+      <c r="X63" s="70"/>
+      <c r="Y63" s="70"/>
+      <c r="Z63" s="70"/>
+      <c r="AA63" s="70">
         <v>53</v>
       </c>
-      <c r="AB63" s="67"/>
-      <c r="AC63" s="67"/>
-      <c r="AD63" s="67"/>
-      <c r="AE63" s="67"/>
-      <c r="AF63" s="67"/>
-      <c r="AG63" s="67"/>
-      <c r="AH63" s="67"/>
-      <c r="AI63" s="67" t="s">
+      <c r="AB63" s="70"/>
+      <c r="AC63" s="70"/>
+      <c r="AD63" s="70"/>
+      <c r="AE63" s="70"/>
+      <c r="AF63" s="70"/>
+      <c r="AG63" s="70"/>
+      <c r="AH63" s="70"/>
+      <c r="AI63" s="70" t="s">
         <v>213</v>
       </c>
-      <c r="AJ63" s="67"/>
-      <c r="AK63" s="67"/>
-      <c r="AL63" s="67"/>
-      <c r="AM63" s="67"/>
-      <c r="AN63" s="67"/>
-      <c r="AO63" s="67"/>
-      <c r="AP63" s="67"/>
+      <c r="AJ63" s="70"/>
+      <c r="AK63" s="70"/>
+      <c r="AL63" s="70"/>
+      <c r="AM63" s="70"/>
+      <c r="AN63" s="70"/>
+      <c r="AO63" s="70"/>
+      <c r="AP63" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="99">
-    <mergeCell ref="AI63:AP63"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="C63:J63"/>
-    <mergeCell ref="K63:R63"/>
-    <mergeCell ref="S63:Z63"/>
-    <mergeCell ref="AA63:AH63"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="C57:J57"/>
-    <mergeCell ref="K57:R57"/>
-    <mergeCell ref="S57:Z57"/>
-    <mergeCell ref="C51:J51"/>
-    <mergeCell ref="K51:R51"/>
-    <mergeCell ref="S51:Z51"/>
-    <mergeCell ref="AA51:AH51"/>
-    <mergeCell ref="AI51:AP51"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C45:J45"/>
-    <mergeCell ref="K45:R45"/>
-    <mergeCell ref="S45:Z45"/>
-    <mergeCell ref="AA45:AH45"/>
-    <mergeCell ref="K39:R39"/>
-    <mergeCell ref="S39:Z39"/>
-    <mergeCell ref="AA39:AH39"/>
-    <mergeCell ref="AI39:AP39"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:L20"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:L22"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:L14"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:L12"/>
-    <mergeCell ref="X53:AH53"/>
-    <mergeCell ref="X41:AH41"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C33:J33"/>
-    <mergeCell ref="K33:R33"/>
-    <mergeCell ref="S33:Z33"/>
-    <mergeCell ref="AA33:AH33"/>
-    <mergeCell ref="C39:J39"/>
-    <mergeCell ref="AI54:AP54"/>
-    <mergeCell ref="C60:J60"/>
-    <mergeCell ref="K60:R60"/>
-    <mergeCell ref="S60:Z60"/>
-    <mergeCell ref="AA60:AH60"/>
-    <mergeCell ref="AI60:AP60"/>
-    <mergeCell ref="C54:J54"/>
-    <mergeCell ref="K54:R54"/>
-    <mergeCell ref="S54:Z54"/>
-    <mergeCell ref="AA54:AH54"/>
-    <mergeCell ref="AA57:AH57"/>
-    <mergeCell ref="AI57:AP57"/>
-    <mergeCell ref="AI42:AP42"/>
-    <mergeCell ref="C48:J48"/>
-    <mergeCell ref="K48:R48"/>
-    <mergeCell ref="S48:Z48"/>
-    <mergeCell ref="AA48:AH48"/>
-    <mergeCell ref="AI48:AP48"/>
-    <mergeCell ref="C42:J42"/>
-    <mergeCell ref="K42:R42"/>
-    <mergeCell ref="S42:Z42"/>
-    <mergeCell ref="AA42:AH42"/>
-    <mergeCell ref="AI45:AP45"/>
     <mergeCell ref="E10:L10"/>
     <mergeCell ref="E15:L16"/>
     <mergeCell ref="E17:L18"/>
@@ -6312,6 +6228,91 @@
     <mergeCell ref="S30:Z30"/>
     <mergeCell ref="AA30:AH30"/>
     <mergeCell ref="AI33:AP33"/>
+    <mergeCell ref="AI42:AP42"/>
+    <mergeCell ref="C48:J48"/>
+    <mergeCell ref="K48:R48"/>
+    <mergeCell ref="S48:Z48"/>
+    <mergeCell ref="AA48:AH48"/>
+    <mergeCell ref="AI48:AP48"/>
+    <mergeCell ref="C42:J42"/>
+    <mergeCell ref="K42:R42"/>
+    <mergeCell ref="S42:Z42"/>
+    <mergeCell ref="AA42:AH42"/>
+    <mergeCell ref="AI45:AP45"/>
+    <mergeCell ref="AI54:AP54"/>
+    <mergeCell ref="C60:J60"/>
+    <mergeCell ref="K60:R60"/>
+    <mergeCell ref="S60:Z60"/>
+    <mergeCell ref="AA60:AH60"/>
+    <mergeCell ref="AI60:AP60"/>
+    <mergeCell ref="C54:J54"/>
+    <mergeCell ref="K54:R54"/>
+    <mergeCell ref="S54:Z54"/>
+    <mergeCell ref="AA54:AH54"/>
+    <mergeCell ref="AA57:AH57"/>
+    <mergeCell ref="AI57:AP57"/>
+    <mergeCell ref="X41:AH41"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="K33:R33"/>
+    <mergeCell ref="S33:Z33"/>
+    <mergeCell ref="AA33:AH33"/>
+    <mergeCell ref="C39:J39"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:L12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:L14"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:L22"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:L20"/>
+    <mergeCell ref="K39:R39"/>
+    <mergeCell ref="S39:Z39"/>
+    <mergeCell ref="AA39:AH39"/>
+    <mergeCell ref="AI39:AP39"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="AA51:AH51"/>
+    <mergeCell ref="AI51:AP51"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C45:J45"/>
+    <mergeCell ref="K45:R45"/>
+    <mergeCell ref="S45:Z45"/>
+    <mergeCell ref="AA45:AH45"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="C57:J57"/>
+    <mergeCell ref="K57:R57"/>
+    <mergeCell ref="S57:Z57"/>
+    <mergeCell ref="C51:J51"/>
+    <mergeCell ref="K51:R51"/>
+    <mergeCell ref="S51:Z51"/>
+    <mergeCell ref="X53:AH53"/>
+    <mergeCell ref="AI63:AP63"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="C63:J63"/>
+    <mergeCell ref="K63:R63"/>
+    <mergeCell ref="S63:Z63"/>
+    <mergeCell ref="AA63:AH63"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>